<commit_message>
feat(FN-997): add test for password protected file and fix merge conflict error
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Documents\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19F7302-3D3A-4BFA-9416-DBAC0FA159DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6AC15-616B-478F-92A4-0D840031E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Facility limit</t>
   </si>
   <si>
-    <t>Facility utilisatin</t>
-  </si>
-  <si>
     <t>Total fees accrued for the month</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Facility utilisation</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +508,7 @@
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="105" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,27 +525,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>20001371</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>20001372</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -588,16 +588,16 @@
     </row>
     <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -606,7 +606,7 @@
         <v>1100627.28</v>
       </c>
       <c r="G4" s="7">
-        <v>124.758</v>
+        <v>124.75</v>
       </c>
       <c r="H4" s="7">
         <v>976.23</v>
@@ -614,16 +614,16 @@
     </row>
     <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>

<commit_message>
feat(fn 997): file type validation and virus scanning (#2152)
Co-authored-by: Christian McCaffery <cmccaffery@ukexportfinance.gov.uk>
</commit_message>
<xml_diff>
--- a/e2e-tests/portal/cypress/fixtures/valid-utilisation-report.xlsx
+++ b/e2e-tests/portal/cypress/fixtures/valid-utilisation-report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CMcCaffery\Documents\Work\dtfs2\e2e-tests\portal\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D19F7302-3D3A-4BFA-9416-DBAC0FA159DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE6AC15-616B-478F-92A4-0D840031E5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{11F33765-8429-4274-B441-B9AF8EF76A44}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Facility limit</t>
   </si>
   <si>
-    <t>Facility utilisatin</t>
-  </si>
-  <si>
     <t>Total fees accrued for the month</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>Facility utilisation</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,7 +508,7 @@
     <col min="8" max="8" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="105" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="87.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,27 +525,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>20001371</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="6">
         <v>600000</v>
@@ -562,16 +562,16 @@
     </row>
     <row r="3" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="4">
         <v>20001372</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
       </c>
       <c r="E3" s="6">
         <v>300000</v>
@@ -588,16 +588,16 @@
     </row>
     <row r="4" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="4">
         <v>20001499</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="E4" s="6">
         <v>1500000</v>
@@ -606,7 +606,7 @@
         <v>1100627.28</v>
       </c>
       <c r="G4" s="7">
-        <v>124.758</v>
+        <v>124.75</v>
       </c>
       <c r="H4" s="7">
         <v>976.23</v>
@@ -614,16 +614,16 @@
     </row>
     <row r="5" spans="1:8" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4">
         <v>20001507</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="E5" s="6">
         <v>2500000</v>

</xml_diff>